<commit_message>
Debug: Fixing the errors
</commit_message>
<xml_diff>
--- a/Default_Inputs.xlsx
+++ b/Default_Inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diane_lab\simple_model\generic_crop_model_project\Git_OOD\Generic-Object-Oriented-Plant-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1454E43C-BCF4-4A48-B207-1D66AC8DEFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CBC352-FF2A-4EE6-BDAF-FE8F87EF8B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{572359C2-A4E8-42F8-B0B6-79384554FF68}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>StartPhotoperiod_Phase</t>
   </si>
@@ -142,6 +141,9 @@
   </si>
   <si>
     <t>Drainage_Factor</t>
+  </si>
+  <si>
+    <t>Soil_Dynamic_Temperature_Factor</t>
   </si>
 </sst>
 </file>
@@ -540,10 +542,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E48718-AB91-4AAB-9B06-8AD4FAA9ABFA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -823,6 +825,14 @@
         <v>0.3</v>
       </c>
     </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>